<commit_message>
Zeiterfassung_Kasper_Christian.xlsx: Erfassung der Zeit des Meetings
Eintragung
</commit_message>
<xml_diff>
--- a/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Kasper_Christian.xlsx
+++ b/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Kasper_Christian.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\RaytRazor\1. Projektplanung\1.1 Zeiterfassung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/kaspch01_hs-ulm_de/Documents/Semester 5/Software Projekt/RaytRazor/1. Projektplanung/1.1 Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C75A2F-0B96-4619-A289-2D4B83601698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{14C75A2F-0B96-4619-A289-2D4B83601698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDCB5944-F73D-4A63-A0C9-5C437BAF975C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" xr2:uid="{A62B9331-51AB-445E-8A86-E52DCE8B38AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21120" xr2:uid="{A62B9331-51AB-445E-8A86-E52DCE8B38AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Name:</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Erster Entwurf</t>
+  </si>
+  <si>
+    <t>Vision, Aufgabenteilung</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -167,12 +170,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,13 +445,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709269E3-F8C7-4951-A5F4-E55A0F95233D}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="2" customWidth="1"/>
@@ -535,7 +535,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+      <c r="A9" s="4">
         <v>45583</v>
       </c>
       <c r="B9" s="2">
@@ -546,6 +546,20 @@
       </c>
       <c r="D9" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>45586</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -557,9 +571,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -707,19 +724,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2314BDC-9EA2-4E30-A7C5-448E8CFAD4C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C634F9CB-9B15-47F9-9574-21334E2C6303}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -743,9 +756,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C634F9CB-9B15-47F9-9574-21334E2C6303}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2314BDC-9EA2-4E30-A7C5-448E8CFAD4C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Zeiterfassung_Kasper_Christian.xlsx: Eintragung der Stunden durchs Meeting
</commit_message>
<xml_diff>
--- a/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Kasper_Christian.xlsx
+++ b/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Kasper_Christian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/kaspch01_hs-ulm_de/Documents/Semester 5/Software Projekt/RaytRazor/1. Projektplanung/1.1 Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{14C75A2F-0B96-4619-A289-2D4B83601698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8C23ADB-CF13-40BB-8A5D-65C64D18524A}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{14C75A2F-0B96-4619-A289-2D4B83601698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C63DCBB4-C19D-4905-ACA3-A8DA0AC952AF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21120" xr2:uid="{A62B9331-51AB-445E-8A86-E52DCE8B38AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Name:</t>
   </si>
@@ -458,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709269E3-F8C7-4951-A5F4-E55A0F95233D}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -631,6 +631,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>45600</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -646,6 +660,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EA32FAADEF28B246BE81F09370D9BDD6" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee5e8cab159ec08823d71aeff920ea58">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcfc458b-b0e2-47b4-8909-d39697dfebcc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6553d0449cd115c0021964cc0df6b6b1" ns2:_="">
     <xsd:import namespace="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
@@ -789,15 +812,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2314BDC-9EA2-4E30-A7C5-448E8CFAD4C2}">
   <ds:schemaRefs>
@@ -808,6 +822,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C634F9CB-9B15-47F9-9574-21334E2C6303}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D748C67-AC05-41D6-A371-F6C56D9D62DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -823,12 +845,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C634F9CB-9B15-47F9-9574-21334E2C6303}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Zeiterfassung_Kasper_Christian.xlsx: Zeiten aufgeschrieben heute und am 12.12.24
</commit_message>
<xml_diff>
--- a/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Kasper_Christian.xlsx
+++ b/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Kasper_Christian.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\CLionProjects\RaytRazor\RaytRazor\1. Projektplanung\1.1 Zeiterfassung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/kaspch01_hs-ulm_de/Documents/Semester 5/Software Projekt/RaytRazor/RaytRazor/1. Projektplanung/1.1 Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6A005C-4933-46F3-BDAF-3A1EB424058A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{2F6A005C-4933-46F3-BDAF-3A1EB424058A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46DD7E8F-F53E-4983-9FB1-1D4159D30B96}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" xr2:uid="{A62B9331-51AB-445E-8A86-E52DCE8B38AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21120" xr2:uid="{A62B9331-51AB-445E-8A86-E52DCE8B38AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>Name:</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Settings-Szene fertiggestellt, Gegenseitige Unterstüzung</t>
+  </si>
+  <si>
+    <t>Importer, Converter</t>
+  </si>
+  <si>
+    <t>Fixxes</t>
+  </si>
+  <si>
+    <t>.obj einlesbar endlich!</t>
   </si>
 </sst>
 </file>
@@ -190,7 +199,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -463,13 +472,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709269E3-F8C7-4951-A5F4-E55A0F95233D}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="2" customWidth="1"/>
@@ -748,6 +757,34 @@
         <v>23</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>45638</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>45665</v>
+      </c>
+      <c r="B24" s="2">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -757,9 +794,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -907,19 +947,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2314BDC-9EA2-4E30-A7C5-448E8CFAD4C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C634F9CB-9B15-47F9-9574-21334E2C6303}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -943,9 +979,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C634F9CB-9B15-47F9-9574-21334E2C6303}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2314BDC-9EA2-4E30-A7C5-448E8CFAD4C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>